<commit_message>
Updated script so it doesn't break
</commit_message>
<xml_diff>
--- a/WPIMatchList.xlsx
+++ b/WPIMatchList.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="10" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name=" 12" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Team Number</t>
   </si>
@@ -90,6 +91,36 @@
   </si>
   <si>
     <t>nope</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Never entered</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hello</t>
   </si>
 </sst>
 </file>
@@ -822,4 +853,736 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="13.7109375"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="8.140625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="1" width="12.85546875"/>
+    <col customWidth="1" max="4" min="4" style="1" width="8.7109375"/>
+    <col customWidth="1" max="5" min="5" style="1" width="10.42578125"/>
+    <col customWidth="1" max="6" min="6" style="1" width="11"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="1" width="16.140625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="1" width="20.140625"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="1" width="20.5703125"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="8.42578125"/>
+    <col customWidth="1" max="11" min="11" style="1" width="20.85546875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>